<commit_message>
final updates for excel files
</commit_message>
<xml_diff>
--- a/history_boys.xlsx
+++ b/history_boys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCland\Desktop\mora9s-hockey-tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4416AE0B-8BE7-427C-B4CA-2C8A805D329C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6634EB-AC9D-4075-A40C-9FDE1D2C346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
   <si>
     <t>Team 1</t>
   </si>
@@ -34,73 +34,61 @@
     <t>Winner</t>
   </si>
   <si>
-    <t>Team A</t>
-  </si>
-  <si>
-    <t>Team C</t>
-  </si>
-  <si>
-    <t>Team E</t>
-  </si>
-  <si>
-    <t>Team G</t>
-  </si>
-  <si>
-    <t>Team B</t>
-  </si>
-  <si>
-    <t>2-3</t>
-  </si>
-  <si>
-    <t>1-1</t>
-  </si>
-  <si>
-    <t>0-5</t>
-  </si>
-  <si>
-    <t>4-1</t>
-  </si>
-  <si>
-    <t>3-1</t>
-  </si>
-  <si>
-    <t>2-2</t>
-  </si>
-  <si>
-    <t>Team D</t>
-  </si>
-  <si>
-    <t>Team F</t>
-  </si>
-  <si>
-    <t>Team H</t>
-  </si>
-  <si>
-    <t>Team I</t>
-  </si>
-  <si>
-    <t>Draw</t>
-  </si>
-  <si>
-    <t>Team XXX</t>
-  </si>
-  <si>
-    <t>7-8</t>
-  </si>
-  <si>
-    <t>12-0</t>
-  </si>
-  <si>
-    <t>Team YYY</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>DEF</t>
-  </si>
-  <si>
-    <t>78-1</t>
+    <t>Mora A</t>
+  </si>
+  <si>
+    <t>Sabra</t>
+  </si>
+  <si>
+    <t>Not Yet Played</t>
+  </si>
+  <si>
+    <t>Pera</t>
+  </si>
+  <si>
+    <t>Wayamba</t>
+  </si>
+  <si>
+    <t>Ruhuna</t>
+  </si>
+  <si>
+    <t>Kelani</t>
+  </si>
+  <si>
+    <t>Japura</t>
+  </si>
+  <si>
+    <t>Colombo</t>
+  </si>
+  <si>
+    <t>Rajarata</t>
+  </si>
+  <si>
+    <t>Mora B</t>
+  </si>
+  <si>
+    <t>MA 1st</t>
+  </si>
+  <si>
+    <t>MB 2nd</t>
+  </si>
+  <si>
+    <t>MB 1st</t>
+  </si>
+  <si>
+    <t>MA 2nd</t>
+  </si>
+  <si>
+    <t>39 Looser</t>
+  </si>
+  <si>
+    <t>40 Looser</t>
+  </si>
+  <si>
+    <t>39 Winner</t>
+  </si>
+  <si>
+    <t>40 Winner</t>
   </si>
 </sst>
 </file>
@@ -469,13 +457,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -496,129 +489,273 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
       <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
matcg mora vs pera
</commit_message>
<xml_diff>
--- a/history_boys.xlsx
+++ b/history_boys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCland\Desktop\mora9s-hockey-tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90B66A6-FE9D-4BA6-ADC3-8996D8FE246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A13365-B2D7-4E0C-96DE-FF16ADDDD07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="30">
   <si>
     <t>Team 1</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>0-2</t>
+  </si>
+  <si>
+    <t>1-1</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +681,10 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>